<commit_message>
Reemplazo de tendencia funcionando
</commit_message>
<xml_diff>
--- a/scripts/dict.xlsx
+++ b/scripts/dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GIT\servel_data\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0F3CB5-D2A2-4DCE-9DA3-E36EDB07EAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B16A8-79C3-4CEC-B3F1-6A78D3F7B0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="columnas" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7015D58-2F88-4AEB-9243-D5CA903F1779}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C53C28-D6A5-4FF2-ADA3-0BEB3C71745D}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TODO check: juntar gráficos
</commit_message>
<xml_diff>
--- a/scripts/dict.xlsx
+++ b/scripts/dict.xlsx
@@ -8,26 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GIT\servel_data\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B16A8-79C3-4CEC-B3F1-6A78D3F7B0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF0B1C4-1BA1-4DB1-873F-9BD374CFF5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="columnas" sheetId="1" r:id="rId1"/>
     <sheet name="valores" sheetId="3" r:id="rId2"/>
     <sheet name="tendencia" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>Archivo</t>
   </si>
@@ -120,6 +130,24 @@
   </si>
   <si>
     <t>votos blancos</t>
+  </si>
+  <si>
+    <t>Elección</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>-1-1</t>
+  </si>
+  <si>
+    <t>Mesa</t>
+  </si>
+  <si>
+    <t>pendiente1</t>
+  </si>
+  <si>
+    <t>pendiente2</t>
   </si>
 </sst>
 </file>
@@ -155,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +469,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +555,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C53C28-D6A5-4FF2-ADA3-0BEB3C71745D}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,4 +809,106 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C0A572-B5EF-4580-97F1-EBBC0DA15BED}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1">
+        <v>-1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <v>161</v>
+      </c>
+      <c r="E2">
+        <f>C2/(C2+D2)</f>
+        <v>0.33195020746887965</v>
+      </c>
+      <c r="F2">
+        <f>D2-C2</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>134</v>
+      </c>
+      <c r="D3">
+        <v>126</v>
+      </c>
+      <c r="E3">
+        <f>C3/(C3+D3)</f>
+        <v>0.51538461538461533</v>
+      </c>
+      <c r="F3">
+        <f>D3-C3</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>F2-F3</f>
+        <v>89</v>
+      </c>
+      <c r="G4">
+        <f>(D3-D2)/(C3-C2)</f>
+        <v>-0.64814814814814814</v>
+      </c>
+      <c r="H4">
+        <f>(C3-C2)/(D3-D2)</f>
+        <v>-1.5428571428571429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Elecciones presidenciales 2021 primera vuelta
</commit_message>
<xml_diff>
--- a/scripts/dict.xlsx
+++ b/scripts/dict.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GIT\servel_data\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A7E899-5DCB-4F60-B06F-D9768BB76F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5DB76F-3088-49A0-A4CE-C7E74F9FF2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="columnas" sheetId="1" r:id="rId1"/>
     <sheet name="valores" sheetId="3" r:id="rId2"/>
     <sheet name="tendencia" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="columnas minimas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="97">
   <si>
     <t>Archivo</t>
   </si>
@@ -132,24 +132,9 @@
     <t>votos blancos</t>
   </si>
   <si>
-    <t>Elección</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>-1-1</t>
-  </si>
-  <si>
     <t>Mesa</t>
   </si>
   <si>
-    <t>pendiente1</t>
-  </si>
-  <si>
-    <t>pendiente2</t>
-  </si>
-  <si>
     <t>Columna</t>
   </si>
   <si>
@@ -265,6 +250,84 @@
   </si>
   <si>
     <t>mesa_electores</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>Nº electores</t>
+  </si>
+  <si>
+    <t>Local de votación</t>
+  </si>
+  <si>
+    <t>Nombre mesa</t>
+  </si>
+  <si>
+    <t>Opción votada</t>
+  </si>
+  <si>
+    <t>Nº de votos en esa opción</t>
+  </si>
+  <si>
+    <t>V o M</t>
+  </si>
+  <si>
+    <t>scraper</t>
+  </si>
+  <si>
+    <t>cod_reg</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>com</t>
+  </si>
+  <si>
+    <t>Minima</t>
+  </si>
+  <si>
+    <t>partido</t>
+  </si>
+  <si>
+    <t>votos_n</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>13-Elecciones Presidenciales, Parlamentarias y de Cores 2021/01-presidenciales-temp.xlsx</t>
+  </si>
+  <si>
+    <t>1. GABRIEL BORIC FONT</t>
+  </si>
+  <si>
+    <t>2. JOSE ANTONIO KAST RIST</t>
+  </si>
+  <si>
+    <t>3. YASNA PROVOSTE CAMPILLAY</t>
+  </si>
+  <si>
+    <t>4. SEBASTIAN SICHEL RAMIREZ</t>
+  </si>
+  <si>
+    <t>5. EDUARDO ARTES BRICHETTI</t>
+  </si>
+  <si>
+    <t>6. MARCO ENRIQUEZ-OMINAMI GUMUCIO</t>
+  </si>
+  <si>
+    <t>7. FRANCO PARISI FERNANDEZ</t>
+  </si>
+  <si>
+    <t>Votos Nulos</t>
+  </si>
+  <si>
+    <t>Votos en Blanco</t>
   </si>
 </sst>
 </file>
@@ -599,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,10 +686,10 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -634,10 +697,10 @@
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -645,65 +708,65 @@
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -711,35 +774,35 @@
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -799,10 +862,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -810,46 +873,46 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -862,7 +925,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,10 +972,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C53C28-D6A5-4FF2-ADA3-0BEB3C71745D}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +991,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -939,10 +1002,10 @@
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -950,10 +1013,10 @@
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -961,10 +1024,10 @@
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -972,10 +1035,10 @@
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D5" s="3">
         <v>-1</v>
@@ -983,10 +1046,10 @@
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D6" s="3">
         <v>-1</v>
@@ -994,18 +1057,18 @@
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1190,10 +1253,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1201,10 +1264,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1212,10 +1275,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1223,10 +1286,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1234,10 +1297,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D31">
         <v>-1</v>
@@ -1245,29 +1308,122 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D32">
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1277,99 +1433,168 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C0A572-B5EF-4580-97F1-EBBC0DA15BED}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1">
-        <v>-1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <v>161</v>
-      </c>
-      <c r="E2">
-        <f>C2/(C2+D2)</f>
-        <v>0.33195020746887965</v>
-      </c>
-      <c r="F2">
-        <f>D2-C2</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>134</v>
-      </c>
-      <c r="D3">
-        <v>126</v>
-      </c>
-      <c r="E3">
-        <f>C3/(C3+D3)</f>
-        <v>0.51538461538461533</v>
-      </c>
-      <c r="F3">
-        <f>D3-C3</f>
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F4">
-        <f>F2-F3</f>
-        <v>89</v>
-      </c>
-      <c r="G4">
-        <f>(D3-D2)/(C3-C2)</f>
-        <v>-0.64814814814814814</v>
-      </c>
-      <c r="H4">
-        <f>(C3-C2)/(D3-D2)</f>
-        <v>-1.5428571428571429</v>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglados algunos bugs, añadida la presidencial (segunda vuelta)
</commit_message>
<xml_diff>
--- a/scripts/dict.xlsx
+++ b/scripts/dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GIT\servel_data\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3DF33C-43E8-462D-802F-113BC9DAFA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735648DE-747A-47B3-9174-FFD81D60C1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="186">
   <si>
     <t>Archivo</t>
   </si>
@@ -589,6 +589,12 @@
   </si>
   <si>
     <t>Elección</t>
+  </si>
+  <si>
+    <t>Resultados_2021_Mesa_PRESIDENCIAL_Tricel_2v_TEMP.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021_presidencial_2v </t>
   </si>
 </sst>
 </file>
@@ -990,29 +996,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A357B1AC-36FD-45D1-B5DC-77BDA1555B76}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5"/>
+    <col min="3" max="3" width="35" style="5" customWidth="1"/>
+    <col min="4" max="4" width="56.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>64</v>
       </c>
@@ -1020,511 +1027,595 @@
         <v>135</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>116</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="3"/>
+      <c r="F4" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>124</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="F11" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>126</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="F13" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>132</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="F17" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>130</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>103</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="F26" s="15" t="s">
         <v>55</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>40</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>163</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="D29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>164</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C30" s="18"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="5" t="s">
+      <c r="C32" s="2"/>
+      <c r="E32" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="C33" s="2"/>
+      <c r="E33" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="C34" s="2"/>
+      <c r="E34" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="C35" s="2"/>
+      <c r="E35" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1536,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F415942-1C64-486A-A17B-F4270AAD8B5F}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,43 +1657,43 @@
         <v>169</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1610,20 +1701,31 @@
         <v>171</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1634,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C53C28-D6A5-4FF2-ADA3-0BEB3C71745D}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,6 +2313,56 @@
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reorden, imágenes, data más actual
</commit_message>
<xml_diff>
--- a/scripts/dict.xlsx
+++ b/scripts/dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GIT\servel_data\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735648DE-747A-47B3-9174-FFD81D60C1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618A9670-DB77-4B2A-8C91-B98925B9C1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="191">
   <si>
     <t>Archivo</t>
   </si>
@@ -595,6 +595,21 @@
   </si>
   <si>
     <t xml:space="preserve">2021_presidencial_2v </t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>2017_presidencial_1v</t>
+  </si>
+  <si>
+    <t>2017_presidencial_2v</t>
+  </si>
+  <si>
+    <t>2021_presidencial_1v</t>
+  </si>
+  <si>
+    <t>2021_presidencial_2v</t>
   </si>
 </sst>
 </file>
@@ -1736,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C53C28-D6A5-4FF2-ADA3-0BEB3C71745D}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,9 +1763,10 @@
     <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>183</v>
       </c>
@@ -1763,8 +1779,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>175</v>
       </c>
@@ -1777,8 +1796,12 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="str">
+        <f>IF(D2=1, "Derecha", IF(D2=-1, "Izquierda", "Sin tendencia"))</f>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>175</v>
       </c>
@@ -1791,8 +1814,12 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="str">
+        <f t="shared" ref="E3:E47" si="0">IF(D3=1, "Derecha", IF(D3=-1, "Izquierda", "Sin tendencia"))</f>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>175</v>
       </c>
@@ -1805,8 +1832,12 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>175</v>
       </c>
@@ -1819,8 +1850,12 @@
       <c r="D5" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>175</v>
       </c>
@@ -1833,8 +1868,12 @@
       <c r="D6" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>175</v>
       </c>
@@ -1844,8 +1883,12 @@
       <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>175</v>
       </c>
@@ -1855,10 +1898,14 @@
       <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -1869,10 +1916,14 @@
       <c r="D9">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
@@ -1883,10 +1934,14 @@
       <c r="D10">
         <v>-1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -1897,10 +1952,14 @@
       <c r="D11">
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
@@ -1911,10 +1970,14 @@
       <c r="D12">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -1925,10 +1988,14 @@
       <c r="D13">
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -1939,10 +2006,14 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
@@ -1953,10 +2024,14 @@
       <c r="D15">
         <v>-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
@@ -1967,10 +2042,14 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
@@ -1978,10 +2057,14 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
@@ -1989,10 +2072,14 @@
       <c r="C18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
@@ -2003,10 +2090,14 @@
       <c r="D19">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
@@ -2017,10 +2108,14 @@
       <c r="D20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2028,10 +2123,14 @@
       <c r="C21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
@@ -2039,8 +2138,12 @@
       <c r="C22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>182</v>
       </c>
@@ -2053,8 +2156,12 @@
       <c r="D23">
         <v>-1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>182</v>
       </c>
@@ -2067,8 +2174,12 @@
       <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>182</v>
       </c>
@@ -2078,8 +2189,12 @@
       <c r="C25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>182</v>
       </c>
@@ -2089,8 +2204,12 @@
       <c r="C26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>176</v>
       </c>
@@ -2103,8 +2222,12 @@
       <c r="D27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>176</v>
       </c>
@@ -2117,8 +2240,12 @@
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>176</v>
       </c>
@@ -2131,8 +2258,12 @@
       <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>176</v>
       </c>
@@ -2145,8 +2276,12 @@
       <c r="D30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>176</v>
       </c>
@@ -2159,8 +2294,12 @@
       <c r="D31">
         <v>-1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>176</v>
       </c>
@@ -2173,8 +2312,12 @@
       <c r="D32">
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>176</v>
       </c>
@@ -2184,8 +2327,12 @@
       <c r="C33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>176</v>
       </c>
@@ -2195,10 +2342,14 @@
       <c r="C34" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
@@ -2209,10 +2360,14 @@
       <c r="D35">
         <v>-1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
@@ -2223,10 +2378,14 @@
       <c r="D36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
@@ -2237,10 +2396,14 @@
       <c r="D37">
         <v>-1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
@@ -2251,10 +2414,14 @@
       <c r="D38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
@@ -2265,10 +2432,14 @@
       <c r="D39">
         <v>-1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
@@ -2279,10 +2450,14 @@
       <c r="D40">
         <v>-1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
@@ -2293,10 +2468,14 @@
       <c r="D41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>7</v>
@@ -2304,10 +2483,14 @@
       <c r="C42" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
@@ -2315,10 +2498,14 @@
       <c r="C43" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
@@ -2329,10 +2516,14 @@
       <c r="D44">
         <v>-1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Izquierda</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>7</v>
@@ -2343,10 +2534,14 @@
       <c r="D45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Derecha</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>7</v>
@@ -2354,16 +2549,24 @@
       <c r="C46" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>75</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sin tendencia</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pre reemplazo de ggplot para mapa por comuna
</commit_message>
<xml_diff>
--- a/scripts/dict.xlsx
+++ b/scripts/dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GIT\servel_data\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618A9670-DB77-4B2A-8C91-B98925B9C1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C61013D-6A72-411B-852D-56ECBF86543C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="229">
   <si>
     <t>Archivo</t>
   </si>
@@ -610,6 +610,120 @@
   </si>
   <si>
     <t>2021_presidencial_2v</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>nombre_formal</t>
+  </si>
+  <si>
+    <t>Presidenciales 2021, primera vuelta</t>
+  </si>
+  <si>
+    <t>Presidenciales 2021, segunda vuelta</t>
+  </si>
+  <si>
+    <t>Sebastian Piñera Echenique</t>
+  </si>
+  <si>
+    <t>Felipe  Kast Sommerhoff</t>
+  </si>
+  <si>
+    <t>Manuel Jose Ossandon Irarrazabal</t>
+  </si>
+  <si>
+    <t>Beatriz  Sanchez Muñoz</t>
+  </si>
+  <si>
+    <t>Alberto  Mayol Miranda</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">Alejandro  Guillier Alvarez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alejandro Navarro Brain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beatriz Sanchez Muñoz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carolina Goic Boroevic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marco  Enriquez-Ominami Gumucio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebastian Piñera Echenique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apruebo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rechazo </t>
+  </si>
+  <si>
+    <t>Joaquin Lavin Infante</t>
+  </si>
+  <si>
+    <t>Ignacio Briones Rojas</t>
+  </si>
+  <si>
+    <t>Sebastian Sichel Ramirez</t>
+  </si>
+  <si>
+    <t>Mario Desbordes Jimenez</t>
+  </si>
+  <si>
+    <t>Gabriel Boric Font</t>
+  </si>
+  <si>
+    <t>Daniel Jadue Jadue</t>
+  </si>
+  <si>
+    <t>José Antonio Kast Rist</t>
+  </si>
+  <si>
+    <t>Yasna Provoste Campillay</t>
+  </si>
+  <si>
+    <t>Sebastián Sichel Ramirez</t>
+  </si>
+  <si>
+    <t>Eduardo Artés Brichetti</t>
+  </si>
+  <si>
+    <t>Marco Enriquez-Ominami Gumucio</t>
+  </si>
+  <si>
+    <t>Franco Parisi Fernandez</t>
+  </si>
+  <si>
+    <t>#e41a1c</t>
+  </si>
+  <si>
+    <t>#377eb8</t>
+  </si>
+  <si>
+    <t>#4daf4a</t>
+  </si>
+  <si>
+    <t>#984ea3</t>
+  </si>
+  <si>
+    <t>#ffff33</t>
+  </si>
+  <si>
+    <t>#ff7f00</t>
+  </si>
+  <si>
+    <t>#a65628</t>
+  </si>
+  <si>
+    <t>#f781bf</t>
   </si>
 </sst>
 </file>
@@ -1011,18 +1125,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A357B1AC-36FD-45D1-B5DC-77BDA1555B76}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
     <col min="4" max="4" width="56.140625" style="5" bestFit="1" customWidth="1"/>
@@ -1595,7 +1709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>160</v>
       </c>
@@ -1610,7 +1724,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>162</v>
       </c>
@@ -1622,7 +1736,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>161</v>
       </c>
@@ -1632,6 +1746,17 @@
       </c>
       <c r="F35" s="6" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1751,9 +1876,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C53C28-D6A5-4FF2-ADA3-0BEB3C71745D}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1764,9 +1889,10 @@
     <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>183</v>
       </c>
@@ -1782,8 +1908,14 @@
       <c r="E1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>175</v>
       </c>
@@ -1800,8 +1932,14 @@
         <f>IF(D2=1, "Derecha", IF(D2=-1, "Izquierda", "Sin tendencia"))</f>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>175</v>
       </c>
@@ -1818,8 +1956,14 @@
         <f t="shared" ref="E3:E47" si="0">IF(D3=1, "Derecha", IF(D3=-1, "Izquierda", "Sin tendencia"))</f>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>175</v>
       </c>
@@ -1836,8 +1980,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>175</v>
       </c>
@@ -1854,8 +2004,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>175</v>
       </c>
@@ -1872,8 +2028,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>175</v>
       </c>
@@ -1887,8 +2049,11 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>175</v>
       </c>
@@ -1902,8 +2067,11 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>187</v>
       </c>
@@ -1920,8 +2088,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>187</v>
       </c>
@@ -1938,8 +2112,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>187</v>
       </c>
@@ -1956,8 +2136,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>187</v>
       </c>
@@ -1974,8 +2160,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>187</v>
       </c>
@@ -1992,8 +2184,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>187</v>
       </c>
@@ -2010,8 +2208,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>187</v>
       </c>
@@ -2028,8 +2232,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>187</v>
       </c>
@@ -2046,8 +2256,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>187</v>
       </c>
@@ -2061,8 +2277,12 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>187</v>
       </c>
@@ -2076,8 +2296,12 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>188</v>
       </c>
@@ -2094,8 +2318,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>188</v>
       </c>
@@ -2112,8 +2342,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>188</v>
       </c>
@@ -2127,8 +2363,11 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>188</v>
       </c>
@@ -2142,8 +2381,11 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>182</v>
       </c>
@@ -2160,8 +2402,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>182</v>
       </c>
@@ -2178,8 +2426,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>182</v>
       </c>
@@ -2193,8 +2447,12 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>182</v>
       </c>
@@ -2208,8 +2466,12 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>176</v>
       </c>
@@ -2226,8 +2488,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>176</v>
       </c>
@@ -2244,8 +2512,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>176</v>
       </c>
@@ -2262,8 +2536,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>176</v>
       </c>
@@ -2280,8 +2560,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>176</v>
       </c>
@@ -2298,8 +2584,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>176</v>
       </c>
@@ -2316,8 +2608,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>176</v>
       </c>
@@ -2331,8 +2629,12 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>176</v>
       </c>
@@ -2346,8 +2648,12 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>189</v>
       </c>
@@ -2364,8 +2670,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>189</v>
       </c>
@@ -2382,8 +2694,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>189</v>
       </c>
@@ -2400,8 +2718,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G37" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>189</v>
       </c>
@@ -2418,8 +2742,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G38" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>189</v>
       </c>
@@ -2436,8 +2766,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G39" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>189</v>
       </c>
@@ -2454,8 +2790,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G40" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>189</v>
       </c>
@@ -2472,8 +2814,14 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G41" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>189</v>
       </c>
@@ -2487,8 +2835,12 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>189</v>
       </c>
@@ -2502,8 +2854,12 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>190</v>
       </c>
@@ -2520,8 +2876,14 @@
         <f t="shared" si="0"/>
         <v>Izquierda</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G44" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>190</v>
       </c>
@@ -2538,8 +2900,14 @@
         <f t="shared" si="0"/>
         <v>Derecha</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G45" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>190</v>
       </c>
@@ -2554,7 +2922,7 @@
         <v>Sin tendencia</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>190</v>
       </c>
@@ -2568,9 +2936,11 @@
         <f t="shared" si="0"/>
         <v>Sin tendencia</v>
       </c>
+      <c r="G47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>